<commit_message>
Trying to fix this BS of format
</commit_message>
<xml_diff>
--- a/bot/menu.xlsx
+++ b/bot/menu.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" state="visible" r:id="rId1"/>
@@ -3560,7 +3560,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
@@ -3568,18 +3568,18 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="17.83203125"/>
     <col customWidth="1" min="3" max="3" width="17"/>
-    <col customWidth="1" min="4" max="4" width="18.83203125"/>
-    <col customWidth="1" min="5" max="5" width="0.33203125"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="24.86328125"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="11.421875"/>
     <col customWidth="1" min="6" max="6" width="18.33203125"/>
-    <col customWidth="1" min="7" max="7" width="0.33203125"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="11.421875"/>
     <col customWidth="1" min="8" max="8" width="18.33203125"/>
     <col customWidth="1" hidden="1" min="9" max="9" width="9.1640625"/>
     <col customWidth="1" min="10" max="10" width="18"/>
     <col customWidth="1" hidden="1" min="11" max="11" width="9.1640625"/>
     <col customWidth="1" min="12" max="12" width="18.1640625"/>
-    <col customWidth="1" min="13" max="13" width="0.33203125"/>
-    <col customWidth="1" min="14" max="14" width="26.6640625"/>
-    <col customWidth="1" min="15" max="15" width="0.5"/>
+    <col customWidth="1" min="13" max="13" width="22.28125"/>
+    <col bestFit="1" customWidth="1" min="14" max="14" width="10.51171875"/>
+    <col customWidth="1" min="15" max="15" width="16.57421875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3591,15 +3591,11 @@
       <c r="D1" s="46">
         <v>45972</v>
       </c>
-      <c r="E1" s="46">
-        <v>45973</v>
-      </c>
+      <c r="E1" s="46"/>
       <c r="F1" s="46">
         <v>45973</v>
       </c>
-      <c r="G1" s="46">
-        <v>45975</v>
-      </c>
+      <c r="G1" s="46"/>
       <c r="H1" s="46">
         <v>45974</v>
       </c>
@@ -3615,12 +3611,13 @@
       <c r="L1" s="46">
         <v>45976</v>
       </c>
-      <c r="M1" s="46">
-        <v>45981</v>
-      </c>
-      <c r="N1" s="46">
-        <v>45977</v>
-      </c>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
     </row>
     <row r="2">
       <c r="A2" s="45"/>
@@ -3631,15 +3628,11 @@
       <c r="D2" s="46">
         <v>46000</v>
       </c>
-      <c r="E2" s="46">
-        <v>46001</v>
-      </c>
+      <c r="E2" s="46"/>
       <c r="F2" s="46">
         <v>46001</v>
       </c>
-      <c r="G2" s="46">
-        <v>46003</v>
-      </c>
+      <c r="G2" s="46"/>
       <c r="H2" s="46">
         <v>46002</v>
       </c>
@@ -3655,12 +3648,8 @@
       <c r="L2" s="46">
         <v>46004</v>
       </c>
-      <c r="M2" s="46">
-        <v>46009</v>
-      </c>
-      <c r="N2" s="46">
-        <v>46005</v>
-      </c>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
     </row>
     <row r="3">
       <c r="A3" s="45"/>
@@ -4535,10 +4524,10 @@
     <col customWidth="1" min="5" max="5" width="18.33203125"/>
     <col customWidth="1" hidden="1" min="6" max="6" width="9.1640625"/>
     <col customWidth="1" min="7" max="7" width="18.5"/>
-    <col customWidth="1" min="8" max="8" width="0.5"/>
-    <col customWidth="1" min="9" max="9" width="20.5"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="11.421875"/>
+    <col customWidth="1" min="9" max="9" width="27.8515625"/>
     <col customWidth="1" hidden="1" min="10" max="10" width="0.1640625"/>
-    <col customWidth="1" min="11" max="11" width="16.83203125"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" width="18.671875"/>
     <col customWidth="1" min="12" max="12" width="14.33203125"/>
     <col customWidth="1" min="13" max="13" width="22.5"/>
   </cols>
@@ -4555,9 +4544,7 @@
       <c r="E1" s="46">
         <v>45979</v>
       </c>
-      <c r="F1" s="46">
-        <v>45981</v>
-      </c>
+      <c r="F1" s="46"/>
       <c r="G1" s="46">
         <v>45980</v>
       </c>
@@ -4567,9 +4554,7 @@
       <c r="I1" s="46">
         <v>45981</v>
       </c>
-      <c r="J1" s="46">
-        <v>45982</v>
-      </c>
+      <c r="J1" s="46"/>
       <c r="K1" s="46">
         <v>45982</v>
       </c>
@@ -4592,15 +4577,11 @@
       <c r="E2" s="46">
         <v>46007</v>
       </c>
-      <c r="F2" s="46">
-        <v>46009</v>
-      </c>
+      <c r="F2" s="46"/>
       <c r="G2" s="46">
         <v>46008</v>
       </c>
-      <c r="H2" s="46">
-        <v>46011</v>
-      </c>
+      <c r="H2" s="46"/>
       <c r="I2" s="46">
         <v>46009</v>
       </c>

</xml_diff>